<commit_message>
Actualización de Sistema y Pruebas
Se actualiza a la última versión trabajada del proyecto y se agregan nuevas pruebas del software en el documento respectivo.
</commit_message>
<xml_diff>
--- a/Pruebas_del_Software.xlsx
+++ b/Pruebas_del_Software.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D-Has\Documents\GitHub\ADSI2067454_ProyectoFormativo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zolrax\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E2C8FF-4BE4-4810-9B7C-734C30BDED72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CDD02F-81E6-410C-980D-803572DF1F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{FB7D6BA0-D0B9-45BE-8122-B1AC8419257E}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="14400" windowHeight="11205" activeTab="1" xr2:uid="{FB7D6BA0-D0B9-45BE-8122-B1AC8419257E}"/>
   </bookViews>
   <sheets>
     <sheet name="Contenido General" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="112">
   <si>
     <t>Lista de Criterios de Evaluación del Software Desarrollado</t>
   </si>
@@ -345,6 +345,27 @@
   </si>
   <si>
     <t>Funcionamiento de iniciar sesion con el usuario recientemente creado  verificado, la sesion se inicializa correctamente y dependiendo el rol, es dirigido a la vista correspondiente.</t>
+  </si>
+  <si>
+    <t>Carlos Noguera</t>
+  </si>
+  <si>
+    <t>Se procede a realizar la respectiva prueba a "Crear Usuario",  el resultado es satisfactorio, se crea correctamente disponiendo de los datos solicitados. Este usuario es guardado satisfactoriamente en la base de datos.</t>
+  </si>
+  <si>
+    <t>Se inicia sesión con el usuario creado, la plataforma no presenta ningún error,  presenta lo correspondiente al rol creado, dando como resultado una prueba satisfactoria. </t>
+  </si>
+  <si>
+    <t>El error presentado anteriormente fue solucionado, al momento de tener un usuario creado, es posible editar datos como correo y rol, además de solo editar el usuario seleccionado, el  error fue totalmente erradicado.</t>
+  </si>
+  <si>
+    <t>Funcionamiento nuevamente comprobado, siendo correcto. La base de datos, recibe y devuelve la infomación de manera satisfactoria.</t>
+  </si>
+  <si>
+    <t>David Gonzalez, Angelica Jimenez, Nelson Merlano, Carlos Noguera</t>
+  </si>
+  <si>
+    <t>La plataforma actualiza sin inconvenientes la información que ya se encuentra dentro dela base de datos, siendo correcto su funcionamiento. </t>
   </si>
 </sst>
 </file>
@@ -649,6 +670,24 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -670,15 +709,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -689,15 +719,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1289,8 +1310,8 @@
   </sheetPr>
   <dimension ref="A2:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21:P21"/>
+    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25:P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,86 +1322,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
     </row>
     <row r="4" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="27" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="27" t="s">
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="27" t="s">
+      <c r="J4" s="34"/>
+      <c r="K4" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="27" t="s">
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="29"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="30" t="s">
+      <c r="R4" s="35"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="U4" s="31"/>
-      <c r="V4" s="32"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="38"/>
     </row>
     <row r="5" spans="1:22" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -1657,34 +1678,34 @@
         <v>44336</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="33" t="s">
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="35"/>
-      <c r="K12" s="33" t="s">
+      <c r="J12" s="28"/>
+      <c r="K12" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="33" t="s">
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="R12" s="34"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="33" t="s">
+      <c r="R12" s="27"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="U12" s="34"/>
-      <c r="V12" s="35"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="28"/>
     </row>
     <row r="13" spans="1:22" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1695,34 +1716,34 @@
         <v>44337</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="33" t="s">
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="33" t="s">
+      <c r="J13" s="28"/>
+      <c r="K13" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="33" t="s">
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="R13" s="34"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="33" t="s">
+      <c r="R13" s="27"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="U13" s="34"/>
-      <c r="V13" s="35"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="28"/>
     </row>
     <row r="14" spans="1:22" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1733,34 +1754,34 @@
         <v>44338</v>
       </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="33" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="35"/>
-      <c r="K14" s="33" t="s">
+      <c r="J14" s="28"/>
+      <c r="K14" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="33" t="s">
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="R14" s="34"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="33" t="s">
+      <c r="R14" s="27"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="U14" s="34"/>
-      <c r="V14" s="35"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="28"/>
     </row>
     <row r="15" spans="1:22" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1915,37 +1936,37 @@
       <c r="V18" s="9"/>
     </row>
     <row r="19" spans="1:22" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="42"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="25">
         <v>44354</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="42"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
       <c r="I19" s="9" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="9"/>
-      <c r="K19" s="33" t="s">
+      <c r="K19" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="40" t="s">
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="R19" s="41"/>
-      <c r="S19" s="42"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="31"/>
       <c r="T19" s="9" t="s">
         <v>45</v>
       </c>
@@ -1953,37 +1974,37 @@
       <c r="V19" s="9"/>
     </row>
     <row r="20" spans="1:22" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="42"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="25">
         <v>44354</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="42"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="9" t="s">
         <v>18</v>
       </c>
       <c r="J20" s="9"/>
-      <c r="K20" s="33" t="s">
+      <c r="K20" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="40" t="s">
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="R20" s="41"/>
-      <c r="S20" s="42"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="31"/>
       <c r="T20" s="9" t="s">
         <v>45</v>
       </c>
@@ -2066,82 +2087,124 @@
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
     </row>
-    <row r="23" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="40"/>
-      <c r="U23" s="41"/>
-      <c r="V23" s="42"/>
-    </row>
-    <row r="24" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="41"/>
-      <c r="V24" s="42"/>
-    </row>
-    <row r="25" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+    <row r="23" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="25">
+        <v>44355</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="U23" s="30"/>
+      <c r="V23" s="31"/>
+    </row>
+    <row r="24" spans="1:22" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="25">
+        <v>44355</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="U24" s="30"/>
+      <c r="V24" s="31"/>
+    </row>
+    <row r="25" spans="1:22" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+      <c r="C25" s="25">
+        <v>44355</v>
+      </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
+      <c r="I25" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="J25" s="9"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="9"/>
+      <c r="K25" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
+      <c r="T25" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="U25" s="30"/>
+      <c r="V25" s="31"/>
     </row>
     <row r="26" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -2149,18 +2212,18 @@
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="28"/>
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="31"/>
     </row>
     <row r="27" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -2464,70 +2527,70 @@
   </sheetPr>
   <dimension ref="A2:V21"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14:S14"/>
+    <sheetView topLeftCell="G10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
     </row>
     <row r="3" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36" t="s">
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36" t="s">
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="37" t="s">
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="38"/>
-      <c r="V3" s="39"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="42"/>
     </row>
     <row r="4" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
@@ -2889,53 +2952,77 @@
       <c r="U13" s="24"/>
       <c r="V13" s="24"/>
     </row>
-    <row r="14" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+    <row r="14" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>44356</v>
+      </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="K14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>92</v>
+      </c>
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
+      <c r="O14" s="24" t="s">
+        <v>109</v>
+      </c>
       <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
       <c r="S14" s="24"/>
-      <c r="T14" s="33"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="35"/>
-    </row>
-    <row r="15" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="T14" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+    </row>
+    <row r="15" spans="1:22" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>44356</v>
+      </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>95</v>
+      </c>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
+      <c r="O15" s="24" t="s">
+        <v>111</v>
+      </c>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="33"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="35"/>
+      <c r="T15" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
     </row>
     <row r="16" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -2957,9 +3044,9 @@
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
       <c r="S16" s="24"/>
-      <c r="T16" s="33"/>
-      <c r="U16" s="34"/>
-      <c r="V16" s="35"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="28"/>
     </row>
     <row r="17" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -2981,9 +3068,9 @@
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
       <c r="S17" s="24"/>
-      <c r="T17" s="33"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="35"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="28"/>
     </row>
     <row r="18" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -3005,9 +3092,9 @@
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
       <c r="S18" s="24"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="35"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="28"/>
     </row>
     <row r="19" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -3029,9 +3116,9 @@
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
       <c r="S19" s="24"/>
-      <c r="T19" s="33"/>
-      <c r="U19" s="34"/>
-      <c r="V19" s="35"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="28"/>
     </row>
     <row r="20" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -3053,9 +3140,9 @@
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
       <c r="S20" s="24"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="35"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="28"/>
     </row>
     <row r="21" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -3077,9 +3164,9 @@
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
       <c r="S21" s="24"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="35"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="115">
@@ -3238,26 +3325,26 @@
       <c r="Q2" s="48"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="27" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="27" t="s">
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="27" t="s">
+      <c r="J3" s="35"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="33" t="s">
         <v>26</v>
       </c>
       <c r="M3" s="44"/>
@@ -3289,9 +3376,9 @@
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="42"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="31"/>
     </row>
     <row r="5" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -3311,9 +3398,9 @@
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="42"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="31"/>
     </row>
     <row r="6" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
@@ -3333,9 +3420,9 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="42"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="31"/>
     </row>
     <row r="7" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -3355,9 +3442,9 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="42"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="31"/>
     </row>
     <row r="8" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
@@ -3377,9 +3464,9 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="42"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="31"/>
     </row>
     <row r="9" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
@@ -3399,9 +3486,9 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="42"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="31"/>
     </row>
     <row r="10" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
@@ -3421,9 +3508,9 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="41"/>
-      <c r="T10" s="42"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="31"/>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
@@ -3443,9 +3530,9 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
-      <c r="R11" s="40"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="42"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="31"/>
     </row>
     <row r="12" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -3465,9 +3552,9 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="42"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
@@ -3487,9 +3574,9 @@
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="42"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="31"/>
     </row>
     <row r="14" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
@@ -3509,9 +3596,9 @@
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="42"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="31"/>
     </row>
     <row r="15" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
@@ -3531,9 +3618,9 @@
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="42"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="31"/>
     </row>
     <row r="16" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -3553,9 +3640,9 @@
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
-      <c r="R16" s="40"/>
-      <c r="S16" s="41"/>
-      <c r="T16" s="42"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="31"/>
     </row>
     <row r="17" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -3575,9 +3662,9 @@
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="42"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="31"/>
     </row>
     <row r="18" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -3597,9 +3684,9 @@
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
-      <c r="R18" s="40"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="42"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="31"/>
     </row>
     <row r="19" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -3619,9 +3706,9 @@
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="42"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="31"/>
     </row>
     <row r="20" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -3641,9 +3728,9 @@
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
-      <c r="R20" s="40"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="42"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="31"/>
     </row>
     <row r="21" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
@@ -3663,9 +3750,9 @@
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
-      <c r="R21" s="40"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="42"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="115">
@@ -3833,35 +3920,35 @@
       <c r="S1" s="48"/>
     </row>
     <row r="2" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="27" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="27" t="s">
+      <c r="K2" s="35"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="28"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="34"/>
       <c r="T2" s="43" t="s">
         <v>38</v>
       </c>
@@ -3870,411 +3957,411 @@
     </row>
     <row r="3" spans="1:22" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="40"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="42"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="31"/>
     </row>
     <row r="4" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="42"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="31"/>
     </row>
     <row r="5" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="42"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="31"/>
     </row>
     <row r="6" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="42"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="31"/>
     </row>
     <row r="7" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="40"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="42"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="31"/>
     </row>
     <row r="8" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="49"/>
       <c r="B8" s="50"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="40"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="42"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="31"/>
     </row>
     <row r="9" spans="1:22" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
       <c r="B9" s="50"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="40"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="42"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="31"/>
     </row>
     <row r="10" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="40"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="42"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="31"/>
     </row>
     <row r="11" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="40"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="42"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="31"/>
     </row>
     <row r="12" spans="1:22" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="40"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="42"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="31"/>
     </row>
     <row r="13" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="40"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="42"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="31"/>
     </row>
     <row r="14" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="40"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="42"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="31"/>
     </row>
     <row r="15" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="40"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="42"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="31"/>
     </row>
     <row r="16" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="41"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="40"/>
-      <c r="U16" s="41"/>
-      <c r="V16" s="42"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="31"/>
     </row>
     <row r="17" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="40"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="42"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="31"/>
     </row>
     <row r="18" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="40"/>
-      <c r="U18" s="41"/>
-      <c r="V18" s="42"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="31"/>
     </row>
     <row r="19" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="41"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="40"/>
-      <c r="U19" s="41"/>
-      <c r="V19" s="42"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="109">

</xml_diff>